<commit_message>
Modified Consolidated Excel Sheet
</commit_message>
<xml_diff>
--- a/Interviews_Columns/Consolidated.xlsx
+++ b/Interviews_Columns/Consolidated.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ahmad\LMS\_Project\GIT\PROJECT-E4\Interviews_Columns\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ahmad\Documents\ESIEE\Semester 2\_Project\GIT\Interviews_Columns\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="61">
   <si>
     <t>Column Name</t>
   </si>
@@ -131,9 +131,6 @@
     <t>connection_id</t>
   </si>
   <si>
-    <t>user_id</t>
-  </si>
-  <si>
     <t>connection_date</t>
   </si>
   <si>
@@ -201,6 +198,15 @@
   </si>
   <si>
     <t>{skipped, correct, incorrect, started}</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>userd_id</t>
+  </si>
+  <si>
+    <t>teacher_feedback</t>
   </si>
 </sst>
 </file>
@@ -270,12 +276,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -556,10 +562,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O43"/>
+  <dimension ref="A1:O35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="M26" sqref="M26"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -570,41 +576,41 @@
     <col min="4" max="4" width="15" customWidth="1"/>
     <col min="5" max="5" width="18.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="25.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="32.77734375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="14.88671875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="24.44140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13.88671875" customWidth="1"/>
-    <col min="14" max="14" width="13" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.77734375" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="10.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3" t="s">
+      <c r="B1" s="6"/>
+      <c r="C1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3" t="s">
+      <c r="D1" s="6"/>
+      <c r="E1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3" t="s">
+      <c r="F1" s="6"/>
+      <c r="G1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="K1" s="3" t="s">
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="K1" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="L1" s="3"/>
-      <c r="N1" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="O1" s="3"/>
+      <c r="L1" s="6"/>
+      <c r="N1" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="O1" s="6"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -631,7 +637,7 @@
       <c r="H2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="3" t="s">
         <v>14</v>
       </c>
       <c r="K2" s="1" t="s">
@@ -649,7 +655,10 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
       </c>
       <c r="C3" t="s">
         <v>18</v>
@@ -657,6 +666,12 @@
       <c r="D3" t="s">
         <v>10</v>
       </c>
+      <c r="E3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F3" t="s">
+        <v>58</v>
+      </c>
       <c r="G3" t="s">
         <v>9</v>
       </c>
@@ -667,10 +682,13 @@
         <v>9</v>
       </c>
       <c r="K3" t="s">
-        <v>35</v>
+        <v>34</v>
+      </c>
+      <c r="L3" t="s">
+        <v>10</v>
       </c>
       <c r="N3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="O3" t="s">
         <v>10</v>
@@ -678,7 +696,7 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>38</v>
+        <v>17</v>
       </c>
       <c r="B4" t="s">
         <v>10</v>
@@ -690,25 +708,34 @@
         <v>6</v>
       </c>
       <c r="G4" t="s">
-        <v>11</v>
+        <v>54</v>
       </c>
       <c r="H4" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="I4" t="s">
-        <v>11</v>
+        <v>54</v>
       </c>
       <c r="K4" t="s">
-        <v>34</v>
+        <v>59</v>
+      </c>
+      <c r="L4" t="s">
+        <v>10</v>
       </c>
       <c r="N4" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="O4" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
       <c r="C5" t="s">
         <v>20</v>
       </c>
@@ -716,62 +743,76 @@
         <v>6</v>
       </c>
       <c r="G5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H5" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="I5" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="K5" t="s">
-        <v>36</v>
+        <v>35</v>
+      </c>
+      <c r="L5" t="s">
+        <v>25</v>
       </c>
       <c r="N5" t="s">
-        <v>5</v>
+        <v>55</v>
       </c>
       <c r="O5" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="G6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" t="s">
+        <v>10</v>
+      </c>
+      <c r="I6" t="s">
+        <v>15</v>
+      </c>
+      <c r="N6" t="s">
+        <v>60</v>
+      </c>
+      <c r="O6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="G7" t="s">
         <v>13</v>
       </c>
-      <c r="H6" t="s">
-        <v>6</v>
-      </c>
-      <c r="I6" t="s">
+      <c r="H7" t="s">
+        <v>25</v>
+      </c>
+      <c r="I7" t="s">
         <v>16</v>
       </c>
-      <c r="N6" t="s">
-        <v>53</v>
-      </c>
-      <c r="O6" t="s">
-        <v>10</v>
-      </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D15" s="3"/>
-      <c r="F15" s="3" t="s">
+      <c r="B15" s="6"/>
+      <c r="C15" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D15" s="6"/>
+      <c r="F15" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="G15" s="3"/>
-      <c r="I15" s="3" t="s">
+      <c r="G15" s="6"/>
+      <c r="I15" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="J15" s="3"/>
-      <c r="L15" s="3" t="s">
+      <c r="J15" s="6"/>
+      <c r="L15" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="M15" s="3"/>
+      <c r="M15" s="6"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
@@ -813,7 +854,10 @@
         <v>10</v>
       </c>
       <c r="C17" t="s">
-        <v>37</v>
+        <v>36</v>
+      </c>
+      <c r="D17" t="s">
+        <v>10</v>
       </c>
       <c r="F17" t="s">
         <v>18</v>
@@ -835,6 +879,12 @@
       <c r="B18" t="s">
         <v>10</v>
       </c>
+      <c r="C18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" t="s">
+        <v>10</v>
+      </c>
       <c r="F18" t="s">
         <v>17</v>
       </c>
@@ -850,19 +900,19 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B19" t="s">
         <v>3</v>
       </c>
       <c r="F19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G19" t="s">
         <v>10</v>
       </c>
       <c r="I19" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J19" t="s">
         <v>3</v>
@@ -870,7 +920,7 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B20" t="s">
         <v>3</v>
@@ -884,13 +934,13 @@
       <c r="I20" t="s">
         <v>28</v>
       </c>
-      <c r="J20" s="5" t="s">
+      <c r="J20" s="4" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B21" t="s">
         <v>26</v>
@@ -902,7 +952,7 @@
         <v>26</v>
       </c>
       <c r="I21" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J21" t="s">
         <v>3</v>
@@ -910,7 +960,7 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B22" t="s">
         <v>3</v>
@@ -932,18 +982,18 @@
       <c r="F23" t="s">
         <v>28</v>
       </c>
-      <c r="G23" s="5" t="s">
+      <c r="G23" s="4" t="s">
         <v>26</v>
       </c>
       <c r="I23" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J23" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="F24" s="6" t="s">
+      <c r="F24" s="5" t="s">
         <v>30</v>
       </c>
       <c r="G24" t="s">
@@ -951,7 +1001,7 @@
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="F25" s="6" t="s">
+      <c r="F25" s="5" t="s">
         <v>31</v>
       </c>
       <c r="G25" t="s">
@@ -968,37 +1018,59 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="F27" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G27" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A28" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B28" s="6"/>
       <c r="F28" t="s">
+        <v>47</v>
+      </c>
+      <c r="G28" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F29" t="s">
         <v>48</v>
-      </c>
-      <c r="G28" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="F29" t="s">
-        <v>49</v>
       </c>
       <c r="G29" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>18</v>
+      </c>
+      <c r="B30" t="s">
+        <v>10</v>
+      </c>
       <c r="F30" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G30" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>36</v>
+      </c>
+      <c r="B31" t="s">
+        <v>10</v>
+      </c>
       <c r="F31" t="s">
         <v>5</v>
       </c>
@@ -1007,83 +1079,49 @@
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>42</v>
+      </c>
+      <c r="B32" t="s">
+        <v>10</v>
+      </c>
       <c r="F32" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G32" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>43</v>
+      </c>
+      <c r="B33" t="s">
+        <v>44</v>
+      </c>
+      <c r="C33" t="s">
+        <v>57</v>
+      </c>
       <c r="F33" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G33" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A36" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B36" s="3"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A37" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>18</v>
-      </c>
-      <c r="B38" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>37</v>
-      </c>
-      <c r="B39" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>43</v>
-      </c>
-      <c r="B40" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>44</v>
-      </c>
-      <c r="B41" t="s">
-        <v>45</v>
-      </c>
-      <c r="C41" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>39</v>
-      </c>
-      <c r="B42" t="s">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>38</v>
+      </c>
+      <c r="B34" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
-        <v>57</v>
-      </c>
-      <c r="B43" t="s">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>56</v>
+      </c>
+      <c r="B35" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1091,7 +1129,7 @@
   <mergeCells count="12">
     <mergeCell ref="K1:L1"/>
     <mergeCell ref="L15:M15"/>
-    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A28:B28"/>
     <mergeCell ref="N1:O1"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:D1"/>

</xml_diff>